<commit_message>
11/18/2020 Experiment results were updated.
</commit_message>
<xml_diff>
--- a/output_for_paper/[11-10-2020] Removal Test.xlsx
+++ b/output_for_paper/[11-10-2020] Removal Test.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SW-ML\UCF\SERDP_Emulsion\output_for_paper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{677B7F11-DCE0-46FD-97F2-77EF82CBDB87}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5ABE471-D2FC-4A93-AF57-0462FB7774A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5955" yWindow="4080" windowWidth="13230" windowHeight="9825" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="2" r:id="rId1"/>
     <sheet name="OS" sheetId="4" r:id="rId2"/>
     <sheet name="OV" sheetId="3" r:id="rId3"/>
+    <sheet name="Turbidity" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
 </workbook>
@@ -346,6 +347,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -355,7 +357,6 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="쉼표" xfId="1" builtinId="3"/>
@@ -661,7 +662,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBADDE83-F686-4EC9-9326-F3657D7E1D55}">
   <dimension ref="A1:X31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
@@ -694,10 +695,10 @@
     </row>
     <row r="2" spans="1:24" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4"/>
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="18"/>
+      <c r="C2" s="19"/>
       <c r="D2" s="9" t="s">
         <v>10</v>
       </c>
@@ -758,7 +759,7 @@
     </row>
     <row r="3" spans="1:24" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4"/>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="20" t="s">
         <v>20</v>
       </c>
       <c r="C3" s="10" t="s">
@@ -824,7 +825,7 @@
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
-      <c r="B4" s="19"/>
+      <c r="B4" s="20"/>
       <c r="C4" s="3" t="s">
         <v>21</v>
       </c>
@@ -897,7 +898,7 @@
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
-      <c r="B5" s="19"/>
+      <c r="B5" s="20"/>
       <c r="C5" s="3" t="s">
         <v>30</v>
       </c>
@@ -970,7 +971,7 @@
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
-      <c r="B6" s="19"/>
+      <c r="B6" s="20"/>
       <c r="C6" s="3" t="s">
         <v>29</v>
       </c>
@@ -1046,7 +1047,7 @@
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
-      <c r="B7" s="19"/>
+      <c r="B7" s="20"/>
       <c r="C7" s="3" t="s">
         <v>28</v>
       </c>
@@ -1122,7 +1123,7 @@
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
-      <c r="B8" s="19"/>
+      <c r="B8" s="20"/>
       <c r="C8" s="3" t="s">
         <v>22</v>
       </c>
@@ -1195,7 +1196,7 @@
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
-      <c r="B9" s="19"/>
+      <c r="B9" s="20"/>
       <c r="C9" s="3" t="s">
         <v>27</v>
       </c>
@@ -1268,7 +1269,7 @@
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
-      <c r="B10" s="19"/>
+      <c r="B10" s="20"/>
       <c r="C10" s="3" t="s">
         <v>23</v>
       </c>
@@ -1341,7 +1342,7 @@
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
-      <c r="B11" s="19"/>
+      <c r="B11" s="20"/>
       <c r="C11" s="3" t="s">
         <v>34</v>
       </c>
@@ -1414,7 +1415,7 @@
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
-      <c r="B12" s="19"/>
+      <c r="B12" s="20"/>
       <c r="C12" s="3" t="s">
         <v>35</v>
       </c>
@@ -1487,7 +1488,7 @@
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
-      <c r="B13" s="19"/>
+      <c r="B13" s="20"/>
       <c r="C13" s="3" t="s">
         <v>24</v>
       </c>
@@ -1560,7 +1561,7 @@
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
-      <c r="B14" s="19"/>
+      <c r="B14" s="20"/>
       <c r="C14" s="3" t="s">
         <v>25</v>
       </c>
@@ -1633,7 +1634,7 @@
     </row>
     <row r="15" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4"/>
-      <c r="B15" s="19"/>
+      <c r="B15" s="20"/>
       <c r="C15" s="3" t="s">
         <v>26</v>
       </c>
@@ -1706,7 +1707,7 @@
     </row>
     <row r="16" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
-      <c r="B16" s="17" t="s">
+      <c r="B16" s="18" t="s">
         <v>9</v>
       </c>
       <c r="C16" s="12" t="s">
@@ -1772,7 +1773,7 @@
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
-      <c r="B17" s="17"/>
+      <c r="B17" s="18"/>
       <c r="C17" s="3" t="s">
         <v>21</v>
       </c>
@@ -1845,7 +1846,7 @@
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
-      <c r="B18" s="17"/>
+      <c r="B18" s="18"/>
       <c r="C18" s="3" t="s">
         <v>30</v>
       </c>
@@ -1921,7 +1922,7 @@
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
-      <c r="B19" s="17"/>
+      <c r="B19" s="18"/>
       <c r="C19" s="3" t="s">
         <v>29</v>
       </c>
@@ -1997,7 +1998,7 @@
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
-      <c r="B20" s="17"/>
+      <c r="B20" s="18"/>
       <c r="C20" s="3" t="s">
         <v>28</v>
       </c>
@@ -2070,7 +2071,7 @@
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
-      <c r="B21" s="17"/>
+      <c r="B21" s="18"/>
       <c r="C21" s="3" t="s">
         <v>22</v>
       </c>
@@ -2143,7 +2144,7 @@
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
-      <c r="B22" s="17"/>
+      <c r="B22" s="18"/>
       <c r="C22" s="3" t="s">
         <v>27</v>
       </c>
@@ -2216,7 +2217,7 @@
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
-      <c r="B23" s="17"/>
+      <c r="B23" s="18"/>
       <c r="C23" s="3" t="s">
         <v>23</v>
       </c>
@@ -2289,7 +2290,7 @@
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
-      <c r="B24" s="17"/>
+      <c r="B24" s="18"/>
       <c r="C24" s="3" t="s">
         <v>34</v>
       </c>
@@ -2362,7 +2363,7 @@
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
-      <c r="B25" s="17"/>
+      <c r="B25" s="18"/>
       <c r="C25" s="3" t="s">
         <v>35</v>
       </c>
@@ -2435,7 +2436,7 @@
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
-      <c r="B26" s="17"/>
+      <c r="B26" s="18"/>
       <c r="C26" s="3" t="s">
         <v>24</v>
       </c>
@@ -2508,7 +2509,7 @@
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
-      <c r="B27" s="17"/>
+      <c r="B27" s="18"/>
       <c r="C27" s="3" t="s">
         <v>25</v>
       </c>
@@ -2581,7 +2582,7 @@
     </row>
     <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
-      <c r="B28" s="17"/>
+      <c r="B28" s="18"/>
       <c r="C28" s="3" t="s">
         <v>26</v>
       </c>
@@ -3153,7 +3154,7 @@
       <c r="F1">
         <v>-7.4999999999999997E-3</v>
       </c>
-      <c r="G1" s="20">
+      <c r="G1" s="17">
         <v>-1E-4</v>
       </c>
       <c r="H1">
@@ -3480,6 +3481,369 @@
       </c>
       <c r="I12">
         <v>-2.8999999999999998E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B152D90D-3560-4C3E-89B0-F76FCD9A5D74}">
+  <dimension ref="A1:I12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>1.7899999999999999E-2</v>
+      </c>
+      <c r="B1">
+        <v>1.84E-2</v>
+      </c>
+      <c r="C1">
+        <v>1.37E-2</v>
+      </c>
+      <c r="D1">
+        <v>1.0699999999999999E-2</v>
+      </c>
+      <c r="E1">
+        <v>1.0800000000000001E-2</v>
+      </c>
+      <c r="F1">
+        <v>1.32E-2</v>
+      </c>
+      <c r="G1">
+        <v>1.9300000000000001E-2</v>
+      </c>
+      <c r="H1">
+        <v>1.9400000000000001E-2</v>
+      </c>
+      <c r="I1">
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="B2">
+        <v>1.66E-2</v>
+      </c>
+      <c r="C2">
+        <v>8.6E-3</v>
+      </c>
+      <c r="D2">
+        <v>8.6999999999999994E-3</v>
+      </c>
+      <c r="E2">
+        <v>9.1000000000000004E-3</v>
+      </c>
+      <c r="F2">
+        <v>1.12E-2</v>
+      </c>
+      <c r="G2">
+        <v>1.6899999999999998E-2</v>
+      </c>
+      <c r="H2">
+        <v>1.7299999999999999E-2</v>
+      </c>
+      <c r="I2">
+        <v>1.32E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1.4200000000000001E-2</v>
+      </c>
+      <c r="B3">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="C3">
+        <v>4.7000000000000002E-3</v>
+      </c>
+      <c r="D3">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E3">
+        <v>2.3E-3</v>
+      </c>
+      <c r="F3">
+        <v>5.1000000000000004E-3</v>
+      </c>
+      <c r="G3">
+        <v>4.0800000000000003E-2</v>
+      </c>
+      <c r="H3">
+        <v>4.0899999999999999E-2</v>
+      </c>
+      <c r="I3">
+        <v>7.7000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1.67E-2</v>
+      </c>
+      <c r="B4">
+        <v>2.7E-2</v>
+      </c>
+      <c r="C4">
+        <v>1.12E-2</v>
+      </c>
+      <c r="D4">
+        <v>8.3000000000000001E-3</v>
+      </c>
+      <c r="E4">
+        <v>9.5999999999999992E-3</v>
+      </c>
+      <c r="F4">
+        <v>1.17E-2</v>
+      </c>
+      <c r="G4">
+        <v>2.76E-2</v>
+      </c>
+      <c r="H4">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="I4">
+        <v>1.6500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>1.6500000000000001E-2</v>
+      </c>
+      <c r="B5">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="C5">
+        <v>6.4000000000000003E-3</v>
+      </c>
+      <c r="D5">
+        <v>3.2000000000000002E-3</v>
+      </c>
+      <c r="E5">
+        <v>5.7999999999999996E-3</v>
+      </c>
+      <c r="F5">
+        <v>9.2999999999999992E-3</v>
+      </c>
+      <c r="G5">
+        <v>4.82E-2</v>
+      </c>
+      <c r="H5">
+        <v>4.8899999999999999E-2</v>
+      </c>
+      <c r="I5">
+        <v>1.8800000000000001E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1.4200000000000001E-2</v>
+      </c>
+      <c r="B6">
+        <v>1.3100000000000001E-2</v>
+      </c>
+      <c r="C6">
+        <v>5.8999999999999999E-3</v>
+      </c>
+      <c r="D6">
+        <v>5.7000000000000002E-3</v>
+      </c>
+      <c r="E6">
+        <v>5.4000000000000003E-3</v>
+      </c>
+      <c r="F6">
+        <v>1.0699999999999999E-2</v>
+      </c>
+      <c r="G6">
+        <v>1.4200000000000001E-2</v>
+      </c>
+      <c r="H6">
+        <v>1.41E-2</v>
+      </c>
+      <c r="I6">
+        <v>1.38E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>9.7999999999999997E-3</v>
+      </c>
+      <c r="B7">
+        <v>1.32E-2</v>
+      </c>
+      <c r="C7">
+        <v>2.2000000000000001E-3</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>8.9999999999999998E-4</v>
+      </c>
+      <c r="F7">
+        <v>7.3000000000000001E-3</v>
+      </c>
+      <c r="G7">
+        <v>1.38E-2</v>
+      </c>
+      <c r="H7">
+        <v>1.41E-2</v>
+      </c>
+      <c r="I7">
+        <v>9.5999999999999992E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1.4E-2</v>
+      </c>
+      <c r="B8">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="C8">
+        <v>7.1000000000000004E-3</v>
+      </c>
+      <c r="D8">
+        <v>4.1999999999999997E-3</v>
+      </c>
+      <c r="E8">
+        <v>1.06E-2</v>
+      </c>
+      <c r="F8">
+        <v>1.34E-2</v>
+      </c>
+      <c r="G8">
+        <v>2.1499999999999998E-2</v>
+      </c>
+      <c r="H8">
+        <v>2.18E-2</v>
+      </c>
+      <c r="I8">
+        <v>1.7600000000000001E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>3.2899999999999999E-2</v>
+      </c>
+      <c r="B9">
+        <v>1.5900000000000001E-2</v>
+      </c>
+      <c r="C9">
+        <v>3.5499999999999997E-2</v>
+      </c>
+      <c r="D9">
+        <v>3.2500000000000001E-2</v>
+      </c>
+      <c r="E9">
+        <v>1.9900000000000001E-2</v>
+      </c>
+      <c r="F9">
+        <v>2.46E-2</v>
+      </c>
+      <c r="G9">
+        <v>1.6400000000000001E-2</v>
+      </c>
+      <c r="H9">
+        <v>1.6500000000000001E-2</v>
+      </c>
+      <c r="I9">
+        <v>3.2000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>4.3E-3</v>
+      </c>
+      <c r="B10">
+        <v>1.4500000000000001E-2</v>
+      </c>
+      <c r="C10">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="D10">
+        <v>5.7999999999999996E-3</v>
+      </c>
+      <c r="E10">
+        <v>2.3E-3</v>
+      </c>
+      <c r="F10">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G10">
+        <v>1.4800000000000001E-2</v>
+      </c>
+      <c r="H10">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="I10">
+        <v>4.3E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>6.0199999999999997E-2</v>
+      </c>
+      <c r="B11">
+        <v>3.3399999999999999E-2</v>
+      </c>
+      <c r="C11">
+        <v>6.6699999999999995E-2</v>
+      </c>
+      <c r="D11">
+        <v>7.2499999999999995E-2</v>
+      </c>
+      <c r="E11">
+        <v>4.3499999999999997E-2</v>
+      </c>
+      <c r="F11">
+        <v>4.0599999999999997E-2</v>
+      </c>
+      <c r="G11">
+        <v>3.3300000000000003E-2</v>
+      </c>
+      <c r="H11">
+        <v>3.3700000000000001E-2</v>
+      </c>
+      <c r="I11">
+        <v>4.3499999999999997E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>1.7299999999999999E-2</v>
+      </c>
+      <c r="B12">
+        <v>1.6899999999999998E-2</v>
+      </c>
+      <c r="C12">
+        <v>1.95E-2</v>
+      </c>
+      <c r="D12">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="E12">
+        <v>8.0999999999999996E-3</v>
+      </c>
+      <c r="F12">
+        <v>0.01</v>
+      </c>
+      <c r="G12">
+        <v>1.7399999999999999E-2</v>
+      </c>
+      <c r="H12">
+        <v>1.7600000000000001E-2</v>
+      </c>
+      <c r="I12">
+        <v>2.07E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>